<commit_message>
Verificación y modificación de target en movimientos
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/consultas/movimientos/ConsultaMovimientos.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/consultas/movimientos/ConsultaMovimientos.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="50">
   <si>
     <t>ID</t>
   </si>
@@ -93,16 +93,19 @@
     <t>ACTIVO</t>
   </si>
   <si>
+    <t>Cuenta Corriente</t>
+  </si>
+  <si>
+    <t>406-140100-05</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>creadoosp11</t>
+  </si>
+  <si>
     <t>Corriente</t>
-  </si>
-  <si>
-    <t>406-140100-01</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>creadoosp11</t>
   </si>
   <si>
     <t>406-101530-07</t>
@@ -172,8 +175,8 @@
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -200,19 +203,81 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -221,7 +286,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -231,13 +296,6 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -251,92 +309,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -349,6 +322,36 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -377,19 +380,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -401,37 +536,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -443,121 +548,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -582,65 +585,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -669,6 +613,39 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -683,152 +660,178 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -849,55 +852,55 @@
   </cellXfs>
   <cellStyles count="50">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="Normal 2" xfId="32"/>
-    <cellStyle name="20% - Accent5" xfId="33" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="34" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="35" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="36" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="37" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="38" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="39" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="40" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="41" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="42" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="43" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="44" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="45" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="46" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="47" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="48" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="49" builtinId="52"/>
+    <cellStyle name="Título 3" xfId="1" builtinId="18"/>
+    <cellStyle name="Moneda [0]" xfId="2" builtinId="7"/>
+    <cellStyle name="40% - Énfasis1" xfId="3" builtinId="31"/>
+    <cellStyle name="Coma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Moneda" xfId="5" builtinId="4"/>
+    <cellStyle name="Coma" xfId="6" builtinId="3"/>
+    <cellStyle name="Porcentaje" xfId="7" builtinId="5"/>
+    <cellStyle name="Hipervínculo" xfId="8" builtinId="8"/>
+    <cellStyle name="Hipervínculo visitado" xfId="9" builtinId="9"/>
+    <cellStyle name="Salida" xfId="10" builtinId="21"/>
+    <cellStyle name="Nota" xfId="11" builtinId="10"/>
+    <cellStyle name="Título 2" xfId="12" builtinId="17"/>
+    <cellStyle name="Texto de advertencia" xfId="13" builtinId="11"/>
+    <cellStyle name="Título" xfId="14" builtinId="15"/>
+    <cellStyle name="Texto explicativo" xfId="15" builtinId="53"/>
+    <cellStyle name="Título 1" xfId="16" builtinId="16"/>
+    <cellStyle name="Título 4" xfId="17" builtinId="19"/>
+    <cellStyle name="Entrada" xfId="18" builtinId="20"/>
+    <cellStyle name="Cálculo" xfId="19" builtinId="22"/>
+    <cellStyle name="Celda de comprobación" xfId="20" builtinId="23"/>
+    <cellStyle name="Celda vinculada" xfId="21" builtinId="24"/>
+    <cellStyle name="Total" xfId="22" builtinId="25"/>
+    <cellStyle name="Correcto" xfId="23" builtinId="26"/>
+    <cellStyle name="40% - Énfasis5" xfId="24" builtinId="47"/>
+    <cellStyle name="Incorrecto" xfId="25" builtinId="27"/>
+    <cellStyle name="Neutro" xfId="26" builtinId="28"/>
+    <cellStyle name="20% - Énfasis5" xfId="27" builtinId="46"/>
+    <cellStyle name="Énfasis1" xfId="28" builtinId="29"/>
+    <cellStyle name="20% - Énfasis1" xfId="29" builtinId="30"/>
+    <cellStyle name="60% - Énfasis1" xfId="30" builtinId="32"/>
+    <cellStyle name="20% - Énfasis6" xfId="31" builtinId="50"/>
+    <cellStyle name="Énfasis2" xfId="32" builtinId="33"/>
+    <cellStyle name="20% - Énfasis2" xfId="33" builtinId="34"/>
+    <cellStyle name="40% - Énfasis2" xfId="34" builtinId="35"/>
+    <cellStyle name="60% - Énfasis2" xfId="35" builtinId="36"/>
+    <cellStyle name="Énfasis3" xfId="36" builtinId="37"/>
+    <cellStyle name="20% - Énfasis3" xfId="37" builtinId="38"/>
+    <cellStyle name="40% - Énfasis3" xfId="38" builtinId="39"/>
+    <cellStyle name="60% - Énfasis3" xfId="39" builtinId="40"/>
+    <cellStyle name="Énfasis4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Énfasis4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Énfasis4" xfId="42" builtinId="43"/>
+    <cellStyle name="60% - Énfasis4" xfId="43" builtinId="44"/>
+    <cellStyle name="Énfasis5" xfId="44" builtinId="45"/>
+    <cellStyle name="60% - Énfasis5" xfId="45" builtinId="48"/>
+    <cellStyle name="Énfasis6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Énfasis6" xfId="47" builtinId="51"/>
+    <cellStyle name="Normal 2" xfId="48"/>
+    <cellStyle name="60% - Énfasis6" xfId="49" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1168,8 +1171,8 @@
   <sheetPr/>
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
@@ -1308,10 +1311,10 @@
         <v>24</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1414,7 +1417,7 @@
         <v>14</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>17</v>
@@ -1441,10 +1444,10 @@
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1506,16 +1509,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1523,50 +1526,50 @@
         <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="2:4">
       <c r="B4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="2:2">
       <c r="B5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="2:2">
       <c r="B6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="2:2">
       <c r="B7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
movimientos tarjeta de crédito
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/consultas/movimientos/ConsultaMovimientos.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/consultas/movimientos/ConsultaMovimientos.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7695"/>
+    <workbookView windowWidth="20490" windowHeight="7695" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Depositos" sheetId="1" r:id="rId1"/>
-    <sheet name="Creditos" sheetId="3" r:id="rId2"/>
+    <sheet name="TarjetasCredito" sheetId="3" r:id="rId2"/>
     <sheet name="Listas" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="49">
   <si>
     <t>ID</t>
   </si>
@@ -111,13 +111,13 @@
     <t>406-101530-07</t>
   </si>
   <si>
-    <t>zrediseño12</t>
-  </si>
-  <si>
-    <t>Prestamo Personal Ta;Prestamo Personal Ta</t>
-  </si>
-  <si>
-    <t>29281005510;29281023970</t>
+    <t>autouser21</t>
+  </si>
+  <si>
+    <t>Tarjetas de credito</t>
+  </si>
+  <si>
+    <t>*6926</t>
   </si>
   <si>
     <t>Orientacion</t>
@@ -136,9 +136,6 @@
   </si>
   <si>
     <t>Detalles</t>
-  </si>
-  <si>
-    <t>Tarjetas de credito</t>
   </si>
   <si>
     <t>Error</t>
@@ -173,8 +170,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -216,6 +213,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -226,67 +238,46 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -309,7 +300,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -323,31 +321,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -380,187 +377,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -589,16 +586,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -615,9 +612,35 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -633,15 +656,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -663,175 +677,158 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1171,8 +1168,8 @@
   <sheetPr/>
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
@@ -1348,8 +1345,8 @@
   <sheetPr/>
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
@@ -1532,44 +1529,44 @@
         <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
         <v>41</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>42</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>43</v>
-      </c>
-      <c r="D3" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="4" spans="2:4">
       <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" t="s">
         <v>45</v>
-      </c>
-      <c r="D4" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="5" spans="2:2">
       <c r="B5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="2:2">
       <c r="B6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="2:2">
       <c r="B7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se finaliza la transacción de consulta de movimientos de E prepago
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/consultas/movimientos/ConsultaMovimientos.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/consultas/movimientos/ConsultaMovimientos.xlsx
@@ -1,32 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26311"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mruiz/Documents/ProyectosTODO1/bancolombia-app-personas-osp-tests-bdd-screen-play/APP_PERSONAS/src/test/resources/datadriven/consultas/movimientos/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="20500" windowHeight="7700" activeTab="1"/>
+    <workbookView windowWidth="20490" windowHeight="7695" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Depositos" sheetId="1" r:id="rId1"/>
     <sheet name="TarjetasCredito" sheetId="3" r:id="rId2"/>
     <sheet name="Inversiones" sheetId="2" r:id="rId3"/>
+    <sheet name="Eprepago" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="43">
   <si>
     <t>ID</t>
   </si>
@@ -124,6 +115,18 @@
     <t>406-725210-11</t>
   </si>
   <si>
+    <t>pagotdc1</t>
+  </si>
+  <si>
+    <t>Personal American Express</t>
+  </si>
+  <si>
+    <t>*0702</t>
+  </si>
+  <si>
+    <t>*1277</t>
+  </si>
+  <si>
     <t>testing10</t>
   </si>
   <si>
@@ -133,35 +136,34 @@
     <t>7001000033569</t>
   </si>
   <si>
-    <t>Personal American Express</t>
-  </si>
-  <si>
-    <t>*0702</t>
-  </si>
-  <si>
-    <t>*1277</t>
-  </si>
-  <si>
-    <t>pagotdc1</t>
+    <t>93221453</t>
+  </si>
+  <si>
+    <t>autotest28</t>
+  </si>
+  <si>
+    <t>MasterCard</t>
+  </si>
+  <si>
+    <t>*5214</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -179,8 +181,159 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,8 +358,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -229,29 +568,318 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="50">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="Normal 2" xfId="32"/>
+    <cellStyle name="20% - Accent5" xfId="33" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="34" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="35" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="36" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="37" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="38" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="39" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="40" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="41" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="42" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="43" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="44" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="45" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="46" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="47" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="48" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="49" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -513,19 +1141,21 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -562,14 +1192,14 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="A2" s="9" t="s">
         <v>14</v>
       </c>
@@ -594,7 +1224,7 @@
       <c r="H2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="8" t="s">
         <v>21</v>
       </c>
       <c r="J2" s="4" t="s">
@@ -613,7 +1243,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="A3" s="9" t="s">
         <v>27</v>
       </c>
@@ -638,7 +1268,7 @@
       <c r="H3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="8" t="s">
         <v>21</v>
       </c>
       <c r="J3" s="4" t="s">
@@ -657,7 +1287,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="A4" s="9" t="s">
         <v>27</v>
       </c>
@@ -682,7 +1312,7 @@
       <c r="H4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="8" t="s">
         <v>21</v>
       </c>
       <c r="J4" s="4" t="s">
@@ -703,20 +1333,22 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -753,14 +1385,14 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="A2" s="9" t="s">
         <v>14</v>
       </c>
@@ -771,7 +1403,7 @@
         <v>14</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>17</v>
@@ -785,7 +1417,7 @@
       <c r="H2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="8" t="s">
         <v>21</v>
       </c>
       <c r="J2" s="4" t="s">
@@ -798,13 +1430,13 @@
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="A3" s="9" t="s">
         <v>27</v>
       </c>
@@ -815,7 +1447,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>17</v>
@@ -829,7 +1461,7 @@
       <c r="H3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="8" t="s">
         <v>21</v>
       </c>
       <c r="J3" s="4" t="s">
@@ -842,48 +1474,50 @@
         <v>24</v>
       </c>
       <c r="M3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="N3" s="3" t="s">
-        <v>37</v>
-      </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
+    <row r="4" spans="1:12">
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.6666666666667" customWidth="1"/>
+    <col min="2" max="2" width="14.8333333333333" customWidth="1"/>
+    <col min="3" max="3" width="12.1666666666667" customWidth="1"/>
+    <col min="4" max="4" width="17.8333333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -920,14 +1554,14 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="A2" s="9" t="s">
         <v>14</v>
       </c>
@@ -938,7 +1572,7 @@
         <v>14</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>17</v>
@@ -952,7 +1586,7 @@
       <c r="H2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="8" t="s">
         <v>21</v>
       </c>
       <c r="J2" s="4" t="s">
@@ -965,10 +1599,10 @@
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -978,5 +1612,141 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:N4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
avance automatizacion vista carrusel
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/consultas/movimientos/ConsultaMovimientos.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/consultas/movimientos/ConsultaMovimientos.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="50">
   <si>
     <t>ID</t>
   </si>
@@ -154,6 +154,24 @@
   </si>
   <si>
     <t>AHO</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>rangoBusquedaXfecha</t>
+  </si>
+  <si>
+    <t>12 Nov 2019 - 14 Nov 2019</t>
+  </si>
+  <si>
+    <t>700100</t>
+  </si>
+  <si>
+    <t>pruebasregistro48</t>
+  </si>
+  <si>
+    <t>*6136</t>
   </si>
 </sst>
 </file>
@@ -217,7 +235,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -240,12 +258,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -257,6 +286,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -997,19 +1027,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
+    <col min="4" max="4" width="15.625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="22.125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1055,8 +1087,11 @@
       <c r="O1" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:15">
+      <c r="P1" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" s="9" t="s">
         <v>14</v>
       </c>
@@ -1100,8 +1135,9 @@
         <v>41</v>
       </c>
       <c r="O2" s="3"/>
-    </row>
-    <row r="3" spans="1:15">
+      <c r="P2" s="3"/>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3" s="9" t="s">
         <v>27</v>
       </c>
@@ -1147,20 +1183,55 @@
       <c r="O3" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="4" spans="1:15">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
+      <c r="P3" s="3"/>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
correcion transaccion movimientos eprepago
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/consultas/movimientos/ConsultaMovimientos.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/consultas/movimientos/ConsultaMovimientos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\OSP_NEW\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\consultas\movimientos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\TODO1\OSP_NEW\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\consultas\movimientos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="51">
   <si>
     <t>ID</t>
   </si>
@@ -141,9 +141,6 @@
     <t>7001000033569</t>
   </si>
   <si>
-    <t>93221453</t>
-  </si>
-  <si>
     <t>MasterCard</t>
   </si>
   <si>
@@ -172,6 +169,12 @@
   </si>
   <si>
     <t>*6136</t>
+  </si>
+  <si>
+    <t>22452521</t>
+  </si>
+  <si>
+    <t>*7848</t>
   </si>
 </sst>
 </file>
@@ -1029,8 +1032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1085,10 +1088,10 @@
         <v>13</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P1" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -1096,7 +1099,7 @@
         <v>14</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>14</v>
@@ -1129,10 +1132,10 @@
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
@@ -1142,7 +1145,7 @@
         <v>27</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>14</v>
@@ -1175,28 +1178,28 @@
         <v>24</v>
       </c>
       <c r="M3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="N3" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="O3" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P3" s="3"/>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>17</v>
@@ -1223,14 +1226,14 @@
         <v>24</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O4" s="3"/>
       <c r="P4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>